<commit_message>
SCRUM-120 Create new SIQ with new Questions for the customer
</commit_message>
<xml_diff>
--- a/Requirments/SIQ/SIQ.xlsx
+++ b/Requirments/SIQ/SIQ.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arsan\OneDrive\Desktop\upload to git\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ebrahem\ITI45\Car-Purchasing\Requirments\SIQ\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC59D19-AEAA-4130-BE6A-AF401A17D716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="166">
   <si>
     <t>Question</t>
   </si>
@@ -529,12 +530,54 @@
   <si>
     <t>SIQ_ID</t>
   </si>
+  <si>
+    <t>The max age for user is 100 year</t>
+  </si>
+  <si>
+    <t>Contact number must start with 201</t>
+  </si>
+  <si>
+    <t>License expiration date at least the current year at max 3 years from the current year</t>
+  </si>
+  <si>
+    <t>Admin accounts will be 6 accounts and stored in database without registration</t>
+  </si>
+  <si>
+    <t>Car name in search lenghth from 3 - 30 chars</t>
+  </si>
+  <si>
+    <t>the Address follow the same criteria of the advertisement</t>
+  </si>
+  <si>
+    <t>SIQ_74</t>
+  </si>
+  <si>
+    <t>SIQ_75</t>
+  </si>
+  <si>
+    <t>SIQ_76</t>
+  </si>
+  <si>
+    <t>SIQ_77</t>
+  </si>
+  <si>
+    <t>SIQ_78</t>
+  </si>
+  <si>
+    <t>SIQ_79</t>
+  </si>
+  <si>
+    <t>The password in the website show as ****** (hidden)</t>
+  </si>
+  <si>
+    <t>SIQ_80</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -568,6 +611,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -661,7 +710,21 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -951,11 +1014,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D74"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1858,8 +1921,87 @@
       </c>
       <c r="D74" s="7"/>
     </row>
+    <row r="75" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C75" s="2"/>
+      <c r="D75" s="7"/>
+    </row>
+    <row r="76" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="C76" s="2"/>
+      <c r="D76" s="7"/>
+    </row>
+    <row r="77" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="C77" s="2"/>
+      <c r="D77" s="7"/>
+    </row>
+    <row r="78" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C78" s="2"/>
+      <c r="D78" s="7"/>
+    </row>
+    <row r="79" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C79" s="2"/>
+      <c r="D79" s="7"/>
+    </row>
+    <row r="80" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C80" s="2"/>
+      <c r="D80" s="7"/>
+    </row>
+    <row r="81" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C81" s="2"/>
+      <c r="D81" s="7"/>
+    </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="C2:C20">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C75:C81">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
@@ -1868,7 +2010,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C20">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C20 C75:C81" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>